<commit_message>
fix cargue excel procesos-productos
</commit_message>
<xml_diff>
--- a/formatos/Procesos_de_Productos.xlsx
+++ b/formatos/Procesos_de_Productos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BDA6B4-1BAE-4B18-A87B-0A906A483C48}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D9377A-48C5-40C7-B5A2-E48F37FA0146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos x Procesos" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Referencia</t>
   </si>
@@ -40,7 +40,10 @@
     <t xml:space="preserve">Maquina </t>
   </si>
   <si>
-    <t>Unidades/Hora</t>
+    <t>Tiempo Alistamiento</t>
+  </si>
+  <si>
+    <t>Tiempo Operación</t>
   </si>
 </sst>
 </file>
@@ -64,7 +67,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,12 +77,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,10 +93,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,36 +385,39 @@
   <sheetPr codeName="Hoja1">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>